<commit_message>
add comment inside function and test case
</commit_message>
<xml_diff>
--- a/Test document/OSSimulator test case.xlsx
+++ b/Test document/OSSimulator test case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="12435" windowHeight="6990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test classification" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -70,6 +70,34 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>File not found</t>
+  </si>
+  <si>
+    <t>Access deny</t>
+  </si>
+  <si>
+    <t>Blank line after the load address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read line with begin by a period followed by a number </t>
+  </si>
+  <si>
+    <t>file has comment line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read line with begin by a period followed by character </t>
+  </si>
+  <si>
+    <t>1
+100</t>
+  </si>
+  <si>
+    <t>.1000 //change store addres to 1000</t>
+  </si>
+  <si>
+    <t>.abc //invalid</t>
   </si>
 </sst>
 </file>
@@ -160,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -171,6 +199,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3298,14 +3336,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3335,7 +3373,7 @@
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -3346,57 +3384,75 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="str">
+      <c r="A7" s="2">
         <f>IF(B7&lt;&gt;"",COUNTA($B$6:B6),"")</f>
-        <v/>
-      </c>
-      <c r="B7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
+      <c r="A8" s="2">
         <f>IF(B8&lt;&gt;"",COUNTA($B$6:B7),"")</f>
-        <v/>
-      </c>
-      <c r="B8" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f>IF(B9&lt;&gt;"",COUNTA($B$6:B8),"")</f>
-        <v/>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="str">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <f>IF(B10&lt;&gt;"",COUNTA($B$6:B9),"")</f>
-        <v/>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
+      <c r="A11" s="2">
         <f>IF(B11&lt;&gt;"",COUNTA($B$6:B10),"")</f>
-        <v/>
-      </c>
-      <c r="B11" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="str">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f>IF(B12&lt;&gt;"",COUNTA($B$6:B11),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3404,7 +3460,7 @@
         <f>IF(B13&lt;&gt;"",COUNTA($B$6:B12),"")</f>
         <v/>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
@@ -3413,7 +3469,7 @@
         <f>IF(B14&lt;&gt;"",COUNTA($B$6:B13),"")</f>
         <v/>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
@@ -3422,7 +3478,7 @@
         <f>IF(B15&lt;&gt;"",COUNTA($B$6:B14),"")</f>
         <v/>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
@@ -3431,7 +3487,7 @@
         <f>IF(B16&lt;&gt;"",COUNTA($B$6:B15),"")</f>
         <v/>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
@@ -3440,7 +3496,7 @@
         <f>IF(B17&lt;&gt;"",COUNTA($B$6:B16),"")</f>
         <v/>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
@@ -3449,7 +3505,7 @@
         <f>IF(B18&lt;&gt;"",COUNTA($B$6:B17),"")</f>
         <v/>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
@@ -3458,7 +3514,7 @@
         <f>IF(B19&lt;&gt;"",COUNTA($B$6:B18),"")</f>
         <v/>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
@@ -3467,7 +3523,7 @@
         <f>IF(B20&lt;&gt;"",COUNTA($B$6:B19),"")</f>
         <v/>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
@@ -3476,7 +3532,7 @@
         <f>IF(B21&lt;&gt;"",COUNTA($B$6:B20),"")</f>
         <v/>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
@@ -3485,7 +3541,7 @@
         <f>IF(B22&lt;&gt;"",COUNTA($B$6:B21),"")</f>
         <v/>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
@@ -3494,7 +3550,7 @@
         <f>IF(B23&lt;&gt;"",COUNTA($B$6:B22),"")</f>
         <v/>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
@@ -3503,7 +3559,7 @@
         <f>IF(B24&lt;&gt;"",COUNTA($B$6:B23),"")</f>
         <v/>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
@@ -3512,7 +3568,7 @@
         <f>IF(B25&lt;&gt;"",COUNTA($B$6:B24),"")</f>
         <v/>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
@@ -3521,7 +3577,7 @@
         <f>IF(B26&lt;&gt;"",COUNTA($B$6:B25),"")</f>
         <v/>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
@@ -3530,7 +3586,7 @@
         <f>IF(B27&lt;&gt;"",COUNTA($B$6:B26),"")</f>
         <v/>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
@@ -3539,7 +3595,7 @@
         <f>IF(B28&lt;&gt;"",COUNTA($B$6:B27),"")</f>
         <v/>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
@@ -3548,7 +3604,7 @@
         <f>IF(B29&lt;&gt;"",COUNTA($B$6:B28),"")</f>
         <v/>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
@@ -3557,7 +3613,7 @@
         <f>IF(B30&lt;&gt;"",COUNTA($B$6:B29),"")</f>
         <v/>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
@@ -3566,7 +3622,7 @@
         <f>IF(B31&lt;&gt;"",COUNTA($B$6:B30),"")</f>
         <v/>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
@@ -3575,7 +3631,7 @@
         <f>IF(B32&lt;&gt;"",COUNTA($B$6:B31),"")</f>
         <v/>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
@@ -3584,7 +3640,7 @@
         <f>IF(B33&lt;&gt;"",COUNTA($B$6:B32),"")</f>
         <v/>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
@@ -3593,7 +3649,7 @@
         <f>IF(B34&lt;&gt;"",COUNTA($B$6:B33),"")</f>
         <v/>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
@@ -3602,7 +3658,7 @@
         <f>IF(B35&lt;&gt;"",COUNTA($B$6:B34),"")</f>
         <v/>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -3611,7 +3667,7 @@
         <f>IF(B36&lt;&gt;"",COUNTA($B$6:B35),"")</f>
         <v/>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
@@ -3620,7 +3676,7 @@
         <f>IF(B37&lt;&gt;"",COUNTA($B$6:B36),"")</f>
         <v/>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
@@ -3629,7 +3685,7 @@
         <f>IF(B38&lt;&gt;"",COUNTA($B$6:B37),"")</f>
         <v/>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
@@ -3638,7 +3694,7 @@
         <f>IF(B39&lt;&gt;"",COUNTA($B$6:B38),"")</f>
         <v/>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
@@ -3647,7 +3703,7 @@
         <f>IF(B40&lt;&gt;"",COUNTA($B$6:B39),"")</f>
         <v/>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
@@ -3656,7 +3712,7 @@
         <f>IF(B41&lt;&gt;"",COUNTA($B$6:B40),"")</f>
         <v/>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
@@ -3665,7 +3721,7 @@
         <f>IF(B42&lt;&gt;"",COUNTA($B$6:B41),"")</f>
         <v/>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
@@ -3674,7 +3730,7 @@
         <f>IF(B43&lt;&gt;"",COUNTA($B$6:B42),"")</f>
         <v/>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
@@ -3683,7 +3739,7 @@
         <f>IF(B44&lt;&gt;"",COUNTA($B$6:B43),"")</f>
         <v/>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
@@ -3692,7 +3748,7 @@
         <f>IF(B45&lt;&gt;"",COUNTA($B$6:B44),"")</f>
         <v/>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
@@ -3701,7 +3757,7 @@
         <f>IF(B46&lt;&gt;"",COUNTA($B$6:B45),"")</f>
         <v/>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
@@ -3710,7 +3766,7 @@
         <f>IF(B47&lt;&gt;"",COUNTA($B$6:B46),"")</f>
         <v/>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
@@ -3719,7 +3775,7 @@
         <f>IF(B48&lt;&gt;"",COUNTA($B$6:B47),"")</f>
         <v/>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
@@ -3728,7 +3784,7 @@
         <f>IF(B49&lt;&gt;"",COUNTA($B$6:B48),"")</f>
         <v/>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
@@ -3737,7 +3793,7 @@
         <f>IF(B50&lt;&gt;"",COUNTA($B$6:B49),"")</f>
         <v/>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
@@ -3746,7 +3802,7 @@
         <f>IF(B51&lt;&gt;"",COUNTA($B$6:B50),"")</f>
         <v/>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
@@ -3755,7 +3811,7 @@
         <f>IF(B52&lt;&gt;"",COUNTA($B$6:B51),"")</f>
         <v/>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
@@ -3764,7 +3820,7 @@
         <f>IF(B53&lt;&gt;"",COUNTA($B$6:B52),"")</f>
         <v/>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
@@ -3773,7 +3829,7 @@
         <f>IF(B54&lt;&gt;"",COUNTA($B$6:B53),"")</f>
         <v/>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
@@ -3782,7 +3838,7 @@
         <f>IF(B55&lt;&gt;"",COUNTA($B$6:B54),"")</f>
         <v/>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
@@ -3791,7 +3847,7 @@
         <f>IF(B56&lt;&gt;"",COUNTA($B$6:B55),"")</f>
         <v/>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
@@ -3800,7 +3856,7 @@
         <f>IF(B57&lt;&gt;"",COUNTA($B$6:B56),"")</f>
         <v/>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
@@ -3809,7 +3865,7 @@
         <f>IF(B58&lt;&gt;"",COUNTA($B$6:B57),"")</f>
         <v/>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
@@ -3818,7 +3874,7 @@
         <f>IF(B59&lt;&gt;"",COUNTA($B$6:B58),"")</f>
         <v/>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
@@ -3827,7 +3883,7 @@
         <f>IF(B60&lt;&gt;"",COUNTA($B$6:B59),"")</f>
         <v/>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
@@ -3836,7 +3892,7 @@
         <f>IF(B61&lt;&gt;"",COUNTA($B$6:B60),"")</f>
         <v/>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
@@ -3845,7 +3901,7 @@
         <f>IF(B62&lt;&gt;"",COUNTA($B$6:B61),"")</f>
         <v/>
       </c>
-      <c r="B62" s="1"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
@@ -3854,7 +3910,7 @@
         <f>IF(B63&lt;&gt;"",COUNTA($B$6:B62),"")</f>
         <v/>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
@@ -3863,7 +3919,7 @@
         <f>IF(B64&lt;&gt;"",COUNTA($B$6:B63),"")</f>
         <v/>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
@@ -3872,7 +3928,7 @@
         <f>IF(B65&lt;&gt;"",COUNTA($B$6:B64),"")</f>
         <v/>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
@@ -3881,7 +3937,7 @@
         <f>IF(B66&lt;&gt;"",COUNTA($B$6:B65),"")</f>
         <v/>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
@@ -3890,7 +3946,7 @@
         <f>IF(B67&lt;&gt;"",COUNTA($B$6:B66),"")</f>
         <v/>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
@@ -3899,7 +3955,7 @@
         <f>IF(B68&lt;&gt;"",COUNTA($B$6:B67),"")</f>
         <v/>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
@@ -3908,7 +3964,7 @@
         <f>IF(B69&lt;&gt;"",COUNTA($B$6:B68),"")</f>
         <v/>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
@@ -3917,7 +3973,7 @@
         <f>IF(B70&lt;&gt;"",COUNTA($B$6:B69),"")</f>
         <v/>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="8"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
@@ -3926,7 +3982,7 @@
         <f>IF(B71&lt;&gt;"",COUNTA($B$6:B70),"")</f>
         <v/>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
@@ -3935,7 +3991,7 @@
         <f>IF(B72&lt;&gt;"",COUNTA($B$6:B71),"")</f>
         <v/>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
@@ -3944,7 +4000,7 @@
         <f>IF(B73&lt;&gt;"",COUNTA($B$6:B72),"")</f>
         <v/>
       </c>
-      <c r="B73" s="1"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
@@ -3953,7 +4009,7 @@
         <f>IF(B74&lt;&gt;"",COUNTA($B$6:B73),"")</f>
         <v/>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
@@ -3962,7 +4018,7 @@
         <f>IF(B75&lt;&gt;"",COUNTA($B$6:B74),"")</f>
         <v/>
       </c>
-      <c r="B75" s="1"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
@@ -3971,7 +4027,7 @@
         <f>IF(B76&lt;&gt;"",COUNTA($B$6:B75),"")</f>
         <v/>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
@@ -3980,7 +4036,7 @@
         <f>IF(B77&lt;&gt;"",COUNTA($B$6:B76),"")</f>
         <v/>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
@@ -3989,7 +4045,7 @@
         <f>IF(B78&lt;&gt;"",COUNTA($B$6:B77),"")</f>
         <v/>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
@@ -3998,7 +4054,7 @@
         <f>IF(B79&lt;&gt;"",COUNTA($B$6:B78),"")</f>
         <v/>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
@@ -4007,7 +4063,7 @@
         <f>IF(B80&lt;&gt;"",COUNTA($B$6:B79),"")</f>
         <v/>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="8"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
@@ -4016,7 +4072,7 @@
         <f>IF(B81&lt;&gt;"",COUNTA($B$6:B80),"")</f>
         <v/>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="8"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
@@ -4025,7 +4081,7 @@
         <f>IF(B82&lt;&gt;"",COUNTA($B$6:B81),"")</f>
         <v/>
       </c>
-      <c r="B82" s="1"/>
+      <c r="B82" s="8"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
@@ -4034,7 +4090,7 @@
         <f>IF(B83&lt;&gt;"",COUNTA($B$6:B82),"")</f>
         <v/>
       </c>
-      <c r="B83" s="1"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
@@ -4043,7 +4099,7 @@
         <f>IF(B84&lt;&gt;"",COUNTA($B$6:B83),"")</f>
         <v/>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
@@ -4052,7 +4108,7 @@
         <f>IF(B85&lt;&gt;"",COUNTA($B$6:B84),"")</f>
         <v/>
       </c>
-      <c r="B85" s="1"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
@@ -4061,7 +4117,7 @@
         <f>IF(B86&lt;&gt;"",COUNTA($B$6:B85),"")</f>
         <v/>
       </c>
-      <c r="B86" s="1"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
@@ -4070,7 +4126,7 @@
         <f>IF(B87&lt;&gt;"",COUNTA($B$6:B86),"")</f>
         <v/>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
@@ -4079,7 +4135,7 @@
         <f>IF(B88&lt;&gt;"",COUNTA($B$6:B87),"")</f>
         <v/>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
@@ -4088,7 +4144,7 @@
         <f>IF(B89&lt;&gt;"",COUNTA($B$6:B88),"")</f>
         <v/>
       </c>
-      <c r="B89" s="1"/>
+      <c r="B89" s="8"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
@@ -4097,7 +4153,7 @@
         <f>IF(B90&lt;&gt;"",COUNTA($B$6:B89),"")</f>
         <v/>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
@@ -4106,7 +4162,7 @@
         <f>IF(B91&lt;&gt;"",COUNTA($B$6:B90),"")</f>
         <v/>
       </c>
-      <c r="B91" s="1"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
@@ -4115,7 +4171,7 @@
         <f>IF(B92&lt;&gt;"",COUNTA($B$6:B91),"")</f>
         <v/>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="8"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
@@ -4124,7 +4180,7 @@
         <f>IF(B93&lt;&gt;"",COUNTA($B$6:B92),"")</f>
         <v/>
       </c>
-      <c r="B93" s="1"/>
+      <c r="B93" s="8"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
@@ -4133,7 +4189,7 @@
         <f>IF(B94&lt;&gt;"",COUNTA($B$6:B93),"")</f>
         <v/>
       </c>
-      <c r="B94" s="1"/>
+      <c r="B94" s="8"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
@@ -4142,7 +4198,7 @@
         <f>IF(B95&lt;&gt;"",COUNTA($B$6:B94),"")</f>
         <v/>
       </c>
-      <c r="B95" s="1"/>
+      <c r="B95" s="8"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
@@ -4151,7 +4207,7 @@
         <f>IF(B96&lt;&gt;"",COUNTA($B$6:B95),"")</f>
         <v/>
       </c>
-      <c r="B96" s="1"/>
+      <c r="B96" s="8"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
@@ -4160,7 +4216,7 @@
         <f>IF(B97&lt;&gt;"",COUNTA($B$6:B96),"")</f>
         <v/>
       </c>
-      <c r="B97" s="1"/>
+      <c r="B97" s="8"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
@@ -4169,7 +4225,7 @@
         <f>IF(B98&lt;&gt;"",COUNTA($B$6:B97),"")</f>
         <v/>
       </c>
-      <c r="B98" s="1"/>
+      <c r="B98" s="8"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
@@ -4178,7 +4234,7 @@
         <f>IF(B99&lt;&gt;"",COUNTA($B$6:B98),"")</f>
         <v/>
       </c>
-      <c r="B99" s="1"/>
+      <c r="B99" s="8"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
@@ -4187,7 +4243,7 @@
         <f>IF(B100&lt;&gt;"",COUNTA($B$6:B99),"")</f>
         <v/>
       </c>
-      <c r="B100" s="1"/>
+      <c r="B100" s="8"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
@@ -4196,7 +4252,7 @@
         <f>IF(B101&lt;&gt;"",COUNTA($B$6:B100),"")</f>
         <v/>
       </c>
-      <c r="B101" s="1"/>
+      <c r="B101" s="8"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
@@ -4217,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>